<commit_message>
List of Algorithms and their uses.
</commit_message>
<xml_diff>
--- a/algorithms.xlsx
+++ b/algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Standard-DSA-Topics-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47E5A10-AB19-4C22-A087-E067480CD57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A62383-4DBE-4EC6-9E64-33BB07DF54A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33888843-6696-42F7-8745-408B5EF762F1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Algorithm</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/sort-an-array-of-0s-1s-and-2s/</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,10 +609,16 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
List of Algorithm and their uses.
</commit_message>
<xml_diff>
--- a/algorithms.xlsx
+++ b/algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Standard-DSA-Topics-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A62383-4DBE-4EC6-9E64-33BB07DF54A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402BD911-DC3B-4656-ABF4-FA63ED885BED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33888843-6696-42F7-8745-408B5EF762F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{33888843-6696-42F7-8745-408B5EF762F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Algorithm</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Sort array, Find inversion count</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/counting-inversions/</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F74BE3E-7101-4BA2-9F08-15FA5C2AED87}">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,9 +520,10 @@
     <col min="5" max="5" width="13.21875" style="3" customWidth="1"/>
     <col min="6" max="6" width="28" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -538,8 +545,9 @@
       <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -558,8 +566,9 @@
       <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -581,8 +590,9 @@
       <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -605,7 +615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -613,60 +623,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1044,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D661AB68-A1B6-4DC3-B805-C1F39A9468A8}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>